<commit_message>
wrapped up dms steps
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/Rules-Nordic44-to-graphql.xlsx
+++ b/cognite/neat/rules/examples/Rules-Nordic44-to-graphql.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrslivincovs/DevProject/Cognite/projects/neat/dev-data-steps/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E98FE27-3390-8942-98EB-1FFC2AF2887A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86705A77-F150-2A42-ACE9-BF504D04A253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31820" yWindow="8560" windowWidth="35560" windowHeight="23060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31820" yWindow="5740" windowWidth="35560" windowHeight="23060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -771,9 +771,6 @@
     <t>mRID</t>
   </si>
   <si>
-    <t>node</t>
-  </si>
-  <si>
     <t>aliasName</t>
   </si>
   <si>
@@ -784,6 +781,9 @@
   </si>
   <si>
     <t>substation</t>
+  </si>
+  <si>
+    <t>rootNode</t>
   </si>
 </sst>
 </file>
@@ -27319,7 +27319,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27684,7 +27684,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="28" t="s">
@@ -27806,7 +27806,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="25" t="s">
@@ -27932,7 +27932,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>30</v>
@@ -27974,7 +27974,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>33</v>
@@ -28094,7 +28094,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
@@ -28134,7 +28134,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="32" t="s">

</xml_diff>

<commit_message>
Feature create fdm instances (#99)
## [0.24.0] - 24-08-23

### Added

- Generation of DM instances
- `DMSDataModelFromRules`, `GenerateCDFNodesAndEdgesFromGraph`, `UploadCDFNodes` and `UploadCDFEdges` added to step libary

### Improved
- Handling of generation of pydantic model instances in case of incomplete graph instances
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/Rules-Nordic44-to-graphql.xlsx
+++ b/cognite/neat/rules/examples/Rules-Nordic44-to-graphql.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrslivincovs/DevProject/Cognite/projects/neat/dev-data-steps/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E98FE27-3390-8942-98EB-1FFC2AF2887A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86705A77-F150-2A42-ACE9-BF504D04A253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31820" yWindow="8560" windowWidth="35560" windowHeight="23060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31820" yWindow="5740" windowWidth="35560" windowHeight="23060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -771,9 +771,6 @@
     <t>mRID</t>
   </si>
   <si>
-    <t>node</t>
-  </si>
-  <si>
     <t>aliasName</t>
   </si>
   <si>
@@ -784,6 +781,9 @@
   </si>
   <si>
     <t>substation</t>
+  </si>
+  <si>
+    <t>rootNode</t>
   </si>
 </sst>
 </file>
@@ -27319,7 +27319,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27684,7 +27684,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="28" t="s">
@@ -27806,7 +27806,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="25" t="s">
@@ -27932,7 +27932,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>30</v>
@@ -27974,7 +27974,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>33</v>
@@ -28094,7 +28094,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
@@ -28134,7 +28134,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="32" t="s">

</xml_diff>

<commit_message>
Feature better pydantic classes (#159)
* updated rules2pydantic models

* updated tests

* Bump version updated CHANGELOG

* nodes can be generated from views only

* added new test, and logic for default

* added test

* small fixes

* last mod
</commit_message>
<xml_diff>
--- a/cognite/neat/rules/examples/Rules-Nordic44-to-graphql.xlsx
+++ b/cognite/neat/rules/examples/Rules-Nordic44-to-graphql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/cognite/neat/rules/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86705A77-F150-2A42-ACE9-BF504D04A253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7A0B6A-107A-FC4C-AEEE-2EB8970117DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31820" yWindow="5740" windowWidth="35560" windowHeight="23060" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27319,7 +27319,7 @@
   <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28101,7 +28101,7 @@
         <v>28</v>
       </c>
       <c r="E19" s="33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="33">
         <v>1</v>

</xml_diff>